<commit_message>
build bundle from loinc spreadsheet
</commit_message>
<xml_diff>
--- a/loinc.xlsx
+++ b/loinc.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmilius/Documents/src/github-bmilius-nmdp/pytestfhir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B00FAC09-672A-6040-AE24-CF84CC97E7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D614B036-1132-B649-8473-B5BA04316CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loinc" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2441" uniqueCount="2256">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2503" uniqueCount="2274">
   <si>
     <t>Code</t>
   </si>
@@ -6805,12 +6805,66 @@
   </si>
   <si>
     <t>https://www.medicinenet.com/hematocrit/article.htm</t>
+  </si>
+  <si>
+    <t>https://www.medicalnewstoday.com/articles/320987#normal-ranges-and-levels</t>
+  </si>
+  <si>
+    <t>https://healthmatters.io/understand-blood-test-results/band-neutrophils</t>
+  </si>
+  <si>
+    <t>https://www.ucsfhealth.org/medical-tests/blood-differential-test</t>
+  </si>
+  <si>
+    <t>http://www.clinlabnavigator.com/complete-blood-count-cbc.html</t>
+  </si>
+  <si>
+    <t>https://www.mayocliniclabs.com/test-catalog/download-setup.php?format=pdf&amp;unit_code=9184</t>
+  </si>
+  <si>
+    <t>https://www.mayocliniclabs.com/test-catalog/download-setup.php?format=pdf&amp;unit_code=9185</t>
+  </si>
+  <si>
+    <t>https://www.mayocliniclabs.com/test-catalog/download-setup.php?format=pdf&amp;unit_code=9186</t>
+  </si>
+  <si>
+    <t>https://training.seer.cancer.gov/abstracting/procedures/clinical/hematologic/blood.html</t>
+  </si>
+  <si>
+    <t>https://www.medicinenet.com/ferritin_blood_test/article.htm</t>
+  </si>
+  <si>
+    <t>https://www.lls.org/leukemia/acute-myeloid-leukemia/diagnosis#:~:text=Blasts%20are%20normally%201%20to,is%20less%20than%2020%20percent.</t>
+  </si>
+  <si>
+    <t>https://www.mountsinai.org/health-library/tests/albumin-blood-serum-test#:~:text=The%20normal%20range%20is%203.4,vary%20slightly%20among%20different%20laboratories.</t>
+  </si>
+  <si>
+    <t>https://labtestsonline.org/tests/reticulocytes</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/topics/medicine-and-dentistry/prolymphocyte</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/topics/biochemistry-genetics-and-molecular-biology/promonocyte</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>https://www.healthcare.uiowa.edu/path_handbook/handbook/test315.html</t>
+  </si>
+  <si>
+    <t>https://www.cancer.ca/en/cancer-information/cancer-type/multiple-myeloma/multiple-myeloma/the-plasma-cells/?region=on</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/topics/neuroscience/plasma-cell</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -7684,7 +7738,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7866,15 +7920,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5660" ySplit="1360" topLeftCell="A36" activePane="bottomRight"/>
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <pane xSplit="4820" ySplit="1160" activePane="bottomRight"/>
+      <selection sqref="A1:XFD1048576"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E38" sqref="E38"/>
+      <selection pane="bottomLeft" activeCell="B103" sqref="B103"/>
+      <selection pane="bottomRight" activeCell="L69" sqref="L69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7884,7 +7938,7 @@
     <col min="6" max="6" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="46" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>264</v>
       </c>
@@ -7922,7 +7976,7 @@
         <v>2245</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -7945,13 +7999,16 @@
         <v>15</v>
       </c>
       <c r="K2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
@@ -7974,13 +8031,16 @@
         <v>15</v>
       </c>
       <c r="K3">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="M3" t="s">
+        <v>2257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
@@ -8003,13 +8063,16 @@
         <v>15</v>
       </c>
       <c r="K4">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="M4" t="s">
+        <v>2257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -8037,8 +8100,11 @@
       <c r="L5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>2258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
@@ -8066,8 +8132,11 @@
       <c r="L6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+      <c r="M6" t="s">
+        <v>2258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -8095,8 +8164,11 @@
       <c r="L7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>2258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -8118,8 +8190,14 @@
       <c r="G8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
@@ -8141,8 +8219,14 @@
       <c r="G9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -8174,7 +8258,7 @@
         <v>2246</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -8206,7 +8290,7 @@
         <v>2246</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
@@ -8238,7 +8322,7 @@
         <v>2246</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
@@ -8270,7 +8354,7 @@
         <v>2246</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>56</v>
       </c>
@@ -8302,7 +8386,7 @@
         <v>2246</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
@@ -8334,7 +8418,7 @@
         <v>2246</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
@@ -8366,7 +8450,7 @@
         <v>2247</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="153" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>62</v>
       </c>
@@ -8398,7 +8482,7 @@
         <v>2248</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="136" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
@@ -8430,7 +8514,7 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="170" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>66</v>
       </c>
@@ -8462,7 +8546,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>68</v>
       </c>
@@ -8494,7 +8578,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="153" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>70</v>
       </c>
@@ -8526,7 +8610,7 @@
         <v>2251</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
@@ -8558,7 +8642,7 @@
         <v>2252</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="136" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
@@ -8590,7 +8674,7 @@
         <v>2253</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -8622,7 +8706,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
@@ -8644,8 +8728,17 @@
       <c r="G25" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <v>7.4</v>
+      </c>
+      <c r="L25">
+        <v>11.2</v>
+      </c>
+      <c r="M25" t="s">
+        <v>2254</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>78</v>
       </c>
@@ -8668,7 +8761,7 @@
         <v>23</v>
       </c>
       <c r="K26">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L26">
         <v>18</v>
@@ -8677,7 +8770,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>80</v>
       </c>
@@ -8700,7 +8793,7 @@
         <v>23</v>
       </c>
       <c r="K27">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L27">
         <v>18</v>
@@ -8709,7 +8802,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>82</v>
       </c>
@@ -8732,7 +8825,7 @@
         <v>23</v>
       </c>
       <c r="K28">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L28">
         <v>18</v>
@@ -8741,7 +8834,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>84</v>
       </c>
@@ -8764,7 +8857,7 @@
         <v>23</v>
       </c>
       <c r="K29">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L29">
         <v>18</v>
@@ -8773,7 +8866,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>86</v>
       </c>
@@ -8796,7 +8889,7 @@
         <v>23</v>
       </c>
       <c r="K30">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L30">
         <v>18</v>
@@ -8805,7 +8898,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="136" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>88</v>
       </c>
@@ -8828,7 +8921,7 @@
         <v>267</v>
       </c>
       <c r="K31">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="L31">
         <v>180</v>
@@ -8837,7 +8930,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>90</v>
       </c>
@@ -8860,7 +8953,7 @@
         <v>23</v>
       </c>
       <c r="K32">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L32">
         <v>18</v>
@@ -8869,7 +8962,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>92</v>
       </c>
@@ -8901,7 +8994,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>94</v>
       </c>
@@ -8923,8 +9016,17 @@
       <c r="G34" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+      <c r="K34">
+        <v>7.4</v>
+      </c>
+      <c r="L34">
+        <v>11.2</v>
+      </c>
+      <c r="M34" t="s">
+        <v>2254</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>96</v>
       </c>
@@ -8946,8 +9048,17 @@
       <c r="G35" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="K35">
+        <v>7.4</v>
+      </c>
+      <c r="L35">
+        <v>11.2</v>
+      </c>
+      <c r="M35" t="s">
+        <v>2254</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>98</v>
       </c>
@@ -8970,7 +9081,7 @@
         <v>15</v>
       </c>
       <c r="K36">
-        <v>38</v>
+        <v>7.4</v>
       </c>
       <c r="L36">
         <v>54</v>
@@ -8979,7 +9090,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>100</v>
       </c>
@@ -9011,7 +9122,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>102</v>
       </c>
@@ -9043,7 +9154,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>104</v>
       </c>
@@ -9075,7 +9186,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>106</v>
       </c>
@@ -9107,7 +9218,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>108</v>
       </c>
@@ -9139,7 +9250,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>110</v>
       </c>
@@ -9171,7 +9282,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>112</v>
       </c>
@@ -9203,7 +9314,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>114</v>
       </c>
@@ -9235,7 +9346,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>116</v>
       </c>
@@ -9267,7 +9378,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>118</v>
       </c>
@@ -9293,10 +9404,13 @@
         <v>1</v>
       </c>
       <c r="L46">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="M46" t="s">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>120</v>
       </c>
@@ -9322,10 +9436,13 @@
         <v>1</v>
       </c>
       <c r="L47">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="M47" t="s">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>122</v>
       </c>
@@ -9351,10 +9468,13 @@
         <v>1</v>
       </c>
       <c r="L48">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="M48" t="s">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>124</v>
       </c>
@@ -9377,13 +9497,16 @@
         <v>15</v>
       </c>
       <c r="K49">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L49">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="M49" t="s">
+        <v>2246</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>126</v>
       </c>
@@ -9406,13 +9529,16 @@
         <v>15</v>
       </c>
       <c r="K50">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L50">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="M50" t="s">
+        <v>2246</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>128</v>
       </c>
@@ -9435,13 +9561,16 @@
         <v>15</v>
       </c>
       <c r="K51">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L51">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="M51" t="s">
+        <v>2246</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>130</v>
       </c>
@@ -9463,8 +9592,14 @@
       <c r="G52" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>132</v>
       </c>
@@ -9486,8 +9621,14 @@
       <c r="G53" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>134</v>
       </c>
@@ -9513,10 +9654,13 @@
         <v>0</v>
       </c>
       <c r="L54">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="M54" t="s">
+        <v>2260</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>136</v>
       </c>
@@ -9542,10 +9686,13 @@
         <v>0</v>
       </c>
       <c r="L55">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="M55" t="s">
+        <v>2261</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>138</v>
       </c>
@@ -9571,10 +9718,13 @@
         <v>0</v>
       </c>
       <c r="L56">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+        <v>0.01</v>
+      </c>
+      <c r="M56" t="s">
+        <v>2262</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>28</v>
       </c>
@@ -9597,7 +9747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>140</v>
       </c>
@@ -9626,7 +9776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>142</v>
       </c>
@@ -9655,7 +9805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>144</v>
       </c>
@@ -9684,7 +9834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>146</v>
       </c>
@@ -9707,13 +9857,16 @@
         <v>15</v>
       </c>
       <c r="K61">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L61">
         <v>8</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="M61" t="s">
+        <v>2263</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>148</v>
       </c>
@@ -9736,13 +9889,16 @@
         <v>15</v>
       </c>
       <c r="K62">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L62">
         <v>8</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="M62" t="s">
+        <v>2263</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>150</v>
       </c>
@@ -9765,13 +9921,16 @@
         <v>15</v>
       </c>
       <c r="K63">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L63">
         <v>8</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="M63" t="s">
+        <v>2263</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>152</v>
       </c>
@@ -9793,8 +9952,14 @@
       <c r="G64" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>154</v>
       </c>
@@ -9816,8 +9981,14 @@
       <c r="G65" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>156</v>
       </c>
@@ -9846,7 +10017,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>158</v>
       </c>
@@ -9875,7 +10046,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>160</v>
       </c>
@@ -9897,8 +10068,14 @@
       <c r="G68" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>162</v>
       </c>
@@ -9920,8 +10097,14 @@
       <c r="G69" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>164</v>
       </c>
@@ -9950,7 +10133,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>166</v>
       </c>
@@ -9979,7 +10162,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>168</v>
       </c>
@@ -10008,7 +10191,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>170</v>
       </c>
@@ -10037,7 +10220,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>172</v>
       </c>
@@ -10066,7 +10249,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>174</v>
       </c>
@@ -10095,7 +10278,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>176</v>
       </c>
@@ -10124,7 +10307,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>178</v>
       </c>
@@ -10153,7 +10336,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>180</v>
       </c>
@@ -10182,7 +10365,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>182</v>
       </c>
@@ -10204,8 +10387,17 @@
       <c r="G79" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="K79">
+        <v>0.1</v>
+      </c>
+      <c r="L79">
+        <v>1</v>
+      </c>
+      <c r="M79" t="s">
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>184</v>
       </c>
@@ -10227,8 +10419,17 @@
       <c r="G80" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="K80">
+        <v>0.1</v>
+      </c>
+      <c r="L80">
+        <v>1</v>
+      </c>
+      <c r="M80" t="s">
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>186</v>
       </c>
@@ -10250,8 +10451,17 @@
       <c r="G81" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="K81">
+        <v>2</v>
+      </c>
+      <c r="L81">
+        <v>4</v>
+      </c>
+      <c r="M81" t="s">
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>188</v>
       </c>
@@ -10273,8 +10483,17 @@
       <c r="G82" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="K82">
+        <v>2</v>
+      </c>
+      <c r="L82">
+        <v>4</v>
+      </c>
+      <c r="M82" t="s">
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>190</v>
       </c>
@@ -10296,8 +10515,17 @@
       <c r="G83" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+      <c r="K83">
+        <v>9.4</v>
+      </c>
+      <c r="L83">
+        <v>12.3</v>
+      </c>
+      <c r="M83" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>192</v>
       </c>
@@ -10319,8 +10547,17 @@
       <c r="G84" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="K84">
+        <v>9.4</v>
+      </c>
+      <c r="L84">
+        <v>12.3</v>
+      </c>
+      <c r="M84" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>194</v>
       </c>
@@ -10343,13 +10580,16 @@
         <v>19</v>
       </c>
       <c r="K85">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="L85">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+      <c r="M85" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>196</v>
       </c>
@@ -10372,13 +10612,16 @@
         <v>19</v>
       </c>
       <c r="K86">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="L86">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+      <c r="M86" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>198</v>
       </c>
@@ -10401,13 +10644,16 @@
         <v>19</v>
       </c>
       <c r="K87">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="L87">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+      <c r="M87" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>200</v>
       </c>
@@ -10430,13 +10676,16 @@
         <v>19</v>
       </c>
       <c r="K88">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="L88">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+      <c r="M88" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>202</v>
       </c>
@@ -10458,8 +10707,17 @@
       <c r="G89" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="K89">
+        <v>10</v>
+      </c>
+      <c r="L89">
+        <v>60</v>
+      </c>
+      <c r="M89" t="s">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>204</v>
       </c>
@@ -10481,8 +10739,17 @@
       <c r="G90" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="K90">
+        <v>10</v>
+      </c>
+      <c r="L90">
+        <v>60</v>
+      </c>
+      <c r="M90" t="s">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>206</v>
       </c>
@@ -10504,8 +10771,17 @@
       <c r="G91" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="K91">
+        <v>0.1</v>
+      </c>
+      <c r="L91">
+        <v>1</v>
+      </c>
+      <c r="M91" t="s">
+        <v>2269</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>208</v>
       </c>
@@ -10527,8 +10803,17 @@
       <c r="G92" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="K92">
+        <v>0.1</v>
+      </c>
+      <c r="L92">
+        <v>1</v>
+      </c>
+      <c r="M92" t="s">
+        <v>2269</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>210</v>
       </c>
@@ -10550,8 +10835,17 @@
       <c r="G93" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="K93">
+        <v>1</v>
+      </c>
+      <c r="L93">
+        <v>20</v>
+      </c>
+      <c r="M93" t="s">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>212</v>
       </c>
@@ -10573,8 +10867,17 @@
       <c r="G94" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="K94">
+        <v>1</v>
+      </c>
+      <c r="L94">
+        <v>20</v>
+      </c>
+      <c r="M94" t="s">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>214</v>
       </c>
@@ -10596,8 +10899,17 @@
       <c r="G95" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="K95">
+        <v>0.1</v>
+      </c>
+      <c r="L95">
+        <v>1</v>
+      </c>
+      <c r="M95" t="s">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>216</v>
       </c>
@@ -10619,8 +10931,17 @@
       <c r="G96" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="K96">
+        <v>0.1</v>
+      </c>
+      <c r="L96">
+        <v>1</v>
+      </c>
+      <c r="M96" t="s">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>218</v>
       </c>
@@ -10642,8 +10963,17 @@
       <c r="G97" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="K97">
+        <v>2</v>
+      </c>
+      <c r="L97">
+        <v>6</v>
+      </c>
+      <c r="M97" t="s">
+        <v>2271</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>220</v>
       </c>
@@ -10665,8 +10995,17 @@
       <c r="G98" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" ht="136" x14ac:dyDescent="0.2">
+      <c r="K98">
+        <v>2</v>
+      </c>
+      <c r="L98">
+        <v>6</v>
+      </c>
+      <c r="M98" t="s">
+        <v>2271</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>222</v>
       </c>
@@ -10689,7 +11028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>224</v>
       </c>
@@ -10715,10 +11054,13 @@
         <v>4</v>
       </c>
       <c r="L100">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="M100" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>226</v>
       </c>
@@ -10744,10 +11086,13 @@
         <v>4</v>
       </c>
       <c r="L101">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="M101" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>228</v>
       </c>
@@ -10773,10 +11118,13 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="L102">
-        <v>7.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="M102" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>230</v>
       </c>
@@ -10798,8 +11146,17 @@
       <c r="G103" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="104" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="K103">
+        <v>25</v>
+      </c>
+      <c r="L103">
+        <v>75</v>
+      </c>
+      <c r="M103" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>232</v>
       </c>
@@ -10821,8 +11178,17 @@
       <c r="G104" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="105" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="K104">
+        <v>25</v>
+      </c>
+      <c r="L104">
+        <v>75</v>
+      </c>
+      <c r="M104" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>234</v>
       </c>
@@ -10844,8 +11210,17 @@
       <c r="G105" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="K105">
+        <v>25</v>
+      </c>
+      <c r="L105">
+        <v>75</v>
+      </c>
+      <c r="M105" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>24</v>
       </c>
@@ -10867,8 +11242,17 @@
       <c r="G106" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="107" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+      <c r="K106">
+        <v>4</v>
+      </c>
+      <c r="L106">
+        <v>11</v>
+      </c>
+      <c r="M106" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>236</v>
       </c>
@@ -10890,8 +11274,17 @@
       <c r="G107" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="108" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="K107">
+        <v>4</v>
+      </c>
+      <c r="L107">
+        <v>11</v>
+      </c>
+      <c r="M107" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>238</v>
       </c>
@@ -10913,8 +11306,17 @@
       <c r="G108" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="109" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+      <c r="K108">
+        <v>4</v>
+      </c>
+      <c r="L108">
+        <v>11</v>
+      </c>
+      <c r="M108" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>240</v>
       </c>
@@ -10936,8 +11338,17 @@
       <c r="G109" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="110" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+      <c r="K109">
+        <v>4</v>
+      </c>
+      <c r="L109">
+        <v>11</v>
+      </c>
+      <c r="M109" t="s">
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>242</v>
       </c>
@@ -10959,8 +11370,17 @@
       <c r="G110" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="111" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+      <c r="K110">
+        <v>3.4</v>
+      </c>
+      <c r="L110">
+        <v>5.4</v>
+      </c>
+      <c r="M110" t="s">
+        <v>2266</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>244</v>
       </c>
@@ -10982,8 +11402,17 @@
       <c r="G111" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="112" spans="1:12" ht="170" x14ac:dyDescent="0.2">
+      <c r="K111">
+        <v>3.4</v>
+      </c>
+      <c r="L111">
+        <v>5.4</v>
+      </c>
+      <c r="M111" t="s">
+        <v>2266</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>246</v>
       </c>
@@ -11005,8 +11434,17 @@
       <c r="G112" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="K112">
+        <v>3.4</v>
+      </c>
+      <c r="L112">
+        <v>5.4</v>
+      </c>
+      <c r="M112" t="s">
+        <v>2266</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>248</v>
       </c>
@@ -11028,8 +11466,17 @@
       <c r="G113" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="K113">
+        <v>3.4</v>
+      </c>
+      <c r="L113">
+        <v>5.4</v>
+      </c>
+      <c r="M113" t="s">
+        <v>2266</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>250</v>
       </c>
@@ -11051,8 +11498,17 @@
       <c r="G114" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="K114">
+        <v>12</v>
+      </c>
+      <c r="L114">
+        <v>300</v>
+      </c>
+      <c r="M114" t="s">
+        <v>2264</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>252</v>
       </c>
@@ -11074,8 +11530,17 @@
       <c r="G115" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="K115">
+        <v>12</v>
+      </c>
+      <c r="L115">
+        <v>300</v>
+      </c>
+      <c r="M115" t="s">
+        <v>2264</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>254</v>
       </c>
@@ -11097,8 +11562,17 @@
       <c r="G116" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="K116">
+        <v>12</v>
+      </c>
+      <c r="L116">
+        <v>300</v>
+      </c>
+      <c r="M116" t="s">
+        <v>2264</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>256</v>
       </c>
@@ -11120,8 +11594,17 @@
       <c r="G117" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="K117">
+        <v>1</v>
+      </c>
+      <c r="L117">
+        <v>5</v>
+      </c>
+      <c r="M117" t="s">
+        <v>2265</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>258</v>
       </c>
@@ -11143,8 +11626,17 @@
       <c r="G118" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="K118">
+        <v>40</v>
+      </c>
+      <c r="L118">
+        <v>60</v>
+      </c>
+      <c r="M118" t="s">
+        <v>2263</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>260</v>
       </c>
@@ -11166,8 +11658,17 @@
       <c r="G119" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="K119">
+        <v>40</v>
+      </c>
+      <c r="L119">
+        <v>60</v>
+      </c>
+      <c r="M119" t="s">
+        <v>2263</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>262</v>
       </c>
@@ -11188,6 +11689,15 @@
       </c>
       <c r="G120" t="s">
         <v>15</v>
+      </c>
+      <c r="K120">
+        <v>40</v>
+      </c>
+      <c r="L120">
+        <v>60</v>
+      </c>
+      <c r="M120" t="s">
+        <v>2263</v>
       </c>
     </row>
   </sheetData>
@@ -11197,7 +11707,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11217,7 +11727,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>